<commit_message>
Anonymised early detector file
</commit_message>
<xml_diff>
--- a/Results/Early Detector.xlsx
+++ b/Results/Early Detector.xlsx
@@ -14,51 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="22">
   <si>
     <t>Mean</t>
-  </si>
-  <si>
-    <t>SohanK</t>
-  </si>
-  <si>
-    <t>anishashetty</t>
-  </si>
-  <si>
-    <t>rroycho</t>
-  </si>
-  <si>
-    <t>anlawande</t>
-  </si>
-  <si>
-    <t>ptrived</t>
-  </si>
-  <si>
-    <t>krishnatejadinavahi</t>
-  </si>
-  <si>
-    <t>keemen90</t>
-  </si>
-  <si>
-    <t>smruthiEJ</t>
-  </si>
-  <si>
-    <t>RonakNisher</t>
-  </si>
-  <si>
-    <t>juhidesai</t>
-  </si>
-  <si>
-    <t>bhashwanth</t>
-  </si>
-  <si>
-    <t>kumar-utsav</t>
-  </si>
-  <si>
-    <t>rarora4</t>
-  </si>
-  <si>
-    <t>yatish27</t>
   </si>
   <si>
     <t>P1</t>
@@ -107,6 +65,21 @@
   </si>
   <si>
     <t>Deviates from Mean</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>User3</t>
+  </si>
+  <si>
+    <t>User4</t>
+  </si>
+  <si>
+    <t>User5</t>
   </si>
 </sst>
 </file>
@@ -451,24 +424,24 @@
   <dimension ref="A1:C282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,7 +454,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -492,7 +465,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -503,7 +476,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -514,7 +487,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -525,7 +498,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -536,7 +509,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,7 +522,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -560,7 +533,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -571,7 +544,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -582,7 +555,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -593,7 +566,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -604,7 +577,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -617,7 +590,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -628,7 +601,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -639,7 +612,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -650,7 +623,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -661,7 +634,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -672,7 +645,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -685,7 +658,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -696,7 +669,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -707,7 +680,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -718,7 +691,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -729,7 +702,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -740,7 +713,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,7 +726,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -764,7 +737,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -775,7 +748,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -786,7 +759,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -797,7 +770,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -808,7 +781,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -821,7 +794,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -832,7 +805,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -843,7 +816,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -854,7 +827,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -865,7 +838,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -876,7 +849,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -889,7 +862,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -900,7 +873,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -911,7 +884,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -922,7 +895,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -933,7 +906,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -944,7 +917,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -957,7 +930,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -968,7 +941,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -979,7 +952,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B64">
         <v>2</v>
@@ -990,7 +963,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -1001,7 +974,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -1012,7 +985,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1025,7 +998,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -1036,7 +1009,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -1047,7 +1020,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -1058,7 +1031,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -1069,7 +1042,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -1080,7 +1053,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1093,7 +1066,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -1104,7 +1077,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -1115,7 +1088,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -1126,7 +1099,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -1137,7 +1110,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -1148,7 +1121,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1161,7 +1134,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -1172,7 +1145,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -1183,7 +1156,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -1194,7 +1167,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -1205,7 +1178,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -1216,7 +1189,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1229,7 +1202,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -1240,7 +1213,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -1251,7 +1224,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -1262,7 +1235,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -1273,7 +1246,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -1284,12 +1257,12 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -1302,7 +1275,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -1313,7 +1286,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -1324,7 +1297,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -1335,7 +1308,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -1346,7 +1319,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -1357,7 +1330,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1370,7 +1343,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -1381,7 +1354,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -1392,7 +1365,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -1403,7 +1376,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -1414,7 +1387,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B116">
         <v>2</v>
@@ -1425,7 +1398,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -1438,7 +1411,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -1449,7 +1422,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B121">
         <v>3</v>
@@ -1460,7 +1433,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -1471,7 +1444,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -1482,7 +1455,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -1493,7 +1466,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -1506,7 +1479,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -1517,7 +1490,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B129">
         <v>4</v>
@@ -1528,7 +1501,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -1539,7 +1512,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -1550,7 +1523,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -1561,7 +1534,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -1574,7 +1547,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -1585,7 +1558,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B137">
         <v>3</v>
@@ -1596,7 +1569,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -1607,7 +1580,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -1618,7 +1591,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -1629,7 +1602,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -1642,7 +1615,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -1653,7 +1626,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B145">
         <v>3</v>
@@ -1664,7 +1637,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B146">
         <v>2</v>
@@ -1675,7 +1648,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -1686,7 +1659,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B148">
         <v>2</v>
@@ -1697,7 +1670,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -1710,7 +1683,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -1721,7 +1694,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B153">
         <v>3</v>
@@ -1732,7 +1705,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B154">
         <v>2</v>
@@ -1743,7 +1716,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -1754,7 +1727,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B156">
         <v>2</v>
@@ -1765,7 +1738,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -1778,7 +1751,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -1789,7 +1762,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B161">
         <v>3</v>
@@ -1800,7 +1773,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B162">
         <v>2</v>
@@ -1811,7 +1784,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -1822,7 +1795,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B164">
         <v>1</v>
@@ -1833,7 +1806,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -1846,7 +1819,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B168">
         <v>1</v>
@@ -1857,7 +1830,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B169">
         <v>4</v>
@@ -1868,7 +1841,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -1879,7 +1852,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -1890,7 +1863,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -1901,7 +1874,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -1914,7 +1887,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -1925,7 +1898,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B177">
         <v>2</v>
@@ -1936,7 +1909,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -1947,7 +1920,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -1958,7 +1931,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -1969,7 +1942,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -1982,7 +1955,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -1993,7 +1966,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B185">
         <v>2</v>
@@ -2004,7 +1977,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -2015,7 +1988,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -2026,7 +1999,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -2037,7 +2010,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -2050,7 +2023,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -2061,7 +2034,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -2072,7 +2045,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -2083,7 +2056,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -2094,7 +2067,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -2105,12 +2078,12 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -2123,7 +2096,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -2134,7 +2107,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -2145,7 +2118,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B204">
         <v>0</v>
@@ -2156,7 +2129,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -2167,7 +2140,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -2180,7 +2153,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B209">
         <v>2</v>
@@ -2191,7 +2164,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B210">
         <v>0</v>
@@ -2202,7 +2175,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -2213,7 +2186,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -2224,7 +2197,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -2237,7 +2210,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B216">
         <v>6</v>
@@ -2248,7 +2221,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B217">
         <v>2</v>
@@ -2259,7 +2232,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B218">
         <v>2</v>
@@ -2270,7 +2243,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B219">
         <v>4</v>
@@ -2281,7 +2254,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -2294,7 +2267,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B223">
         <v>6</v>
@@ -2305,7 +2278,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B224">
         <v>2</v>
@@ -2316,7 +2289,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B225">
         <v>2</v>
@@ -2327,7 +2300,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B226">
         <v>4</v>
@@ -2338,7 +2311,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -2351,7 +2324,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B230">
         <v>3</v>
@@ -2362,7 +2335,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B231">
         <v>2</v>
@@ -2373,7 +2346,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B232">
         <v>3</v>
@@ -2384,7 +2357,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B233">
         <v>3</v>
@@ -2395,7 +2368,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -2408,7 +2381,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B237">
         <v>3</v>
@@ -2419,7 +2392,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B238">
         <v>2</v>
@@ -2430,7 +2403,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B239">
         <v>3</v>
@@ -2441,7 +2414,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B240">
         <v>3</v>
@@ -2452,7 +2425,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -2465,7 +2438,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B244">
         <v>3</v>
@@ -2476,7 +2449,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B245">
         <v>2</v>
@@ -2487,7 +2460,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B246">
         <v>3</v>
@@ -2498,7 +2471,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B247">
         <v>3</v>
@@ -2509,7 +2482,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -2522,7 +2495,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B251">
         <v>3</v>
@@ -2533,7 +2506,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B252">
         <v>2</v>
@@ -2544,7 +2517,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B253">
         <v>3</v>
@@ -2555,7 +2528,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B254">
         <v>3</v>
@@ -2566,7 +2539,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -2579,7 +2552,7 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B258">
         <v>0</v>
@@ -2590,7 +2563,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B259">
         <v>1</v>
@@ -2601,7 +2574,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B260">
         <v>1</v>
@@ -2612,7 +2585,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B261">
         <v>2</v>
@@ -2623,7 +2596,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -2636,7 +2609,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B265">
         <v>0</v>
@@ -2647,7 +2620,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B266">
         <v>1</v>
@@ -2658,7 +2631,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B267">
         <v>1</v>
@@ -2669,7 +2642,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B268">
         <v>2</v>
@@ -2680,7 +2653,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -2693,7 +2666,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B272">
         <v>0</v>
@@ -2704,7 +2677,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B273">
         <v>0</v>
@@ -2715,7 +2688,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B274">
         <v>0</v>
@@ -2726,7 +2699,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B275">
         <v>0</v>
@@ -2737,7 +2710,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -2750,7 +2723,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B279">
         <v>0</v>
@@ -2761,7 +2734,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B280">
         <v>0</v>
@@ -2772,7 +2745,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B281">
         <v>0</v>
@@ -2783,7 +2756,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B282">
         <v>0</v>

</xml_diff>